<commit_message>
export user dan import, seeder, sudahh
</commit_message>
<xml_diff>
--- a/UserImport.xlsx
+++ b/UserImport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Music\aiagent\presensi-karyawan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3672CA4D-9B4F-4AE6-BEDA-BFCE82A7F16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE80D3D-5EE3-4EF3-B42B-8BA564313A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{CA96A42D-7792-4A95-B395-ACFA30E187D7}"/>
+    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="11520" xr2:uid="{CA96A42D-7792-4A95-B395-ACFA30E187D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,28 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>AMINU BIL HUDA</t>
-  </si>
-  <si>
-    <t>huda@example.com</t>
-  </si>
-  <si>
-    <t>DANANG SUPRIYANTO</t>
-  </si>
-  <si>
-    <t>danang@example.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Staf TU</t>
   </si>
@@ -64,7 +43,49 @@
     <t>Guru</t>
   </si>
   <si>
-    <t>name</t>
+    <t>Nama</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Peran</t>
+  </si>
+  <si>
+    <t>Nomor Telepon</t>
+  </si>
+  <si>
+    <t>Notifikasi WA</t>
+  </si>
+  <si>
+    <t>aminu bil huda</t>
+  </si>
+  <si>
+    <t>aminu@aminu.com</t>
+  </si>
+  <si>
+    <t>aminu</t>
+  </si>
+  <si>
+    <t>Ya</t>
+  </si>
+  <si>
+    <t>danang putra</t>
+  </si>
+  <si>
+    <t>danang@danang.com</t>
+  </si>
+  <si>
+    <t>danang</t>
+  </si>
+  <si>
+    <t>Tidak</t>
   </si>
 </sst>
 </file>
@@ -429,58 +450,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83815C7-08B6-4E2B-9346-1AEF36B5C379}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>12345678</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>85707357080</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>12345678</v>
+      </c>
+      <c r="E3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
+      <c r="F3">
+        <v>897648391</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{8E7E16F0-29C5-44BE-B51F-19441A9A2866}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{D2BEDB5A-59B4-4929-9285-16C1D03B1C3B}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D241BC00-8E66-4883-8451-9C0BB6BB826A}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{B0C165B9-AF90-4807-AED7-07C01A018ECA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>